<commit_message>
Se agrega lista de parametros por default.
</commit_message>
<xml_diff>
--- a/Diagramas/entradas y salidas.xlsx
+++ b/Diagramas/entradas y salidas.xlsx
@@ -1,32 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>P40</t>
   </si>
   <si>
-    <t>P00</t>
-  </si>
-  <si>
-    <t>P01</t>
-  </si>
-  <si>
     <t>HONEYWELL NO HABILITADO</t>
   </si>
   <si>
@@ -90,63 +83,6 @@
     <t>GIRAR CANASTA IZQUIERDA (CONTROL COLGANTE)</t>
   </si>
   <si>
-    <t>P17</t>
-  </si>
-  <si>
-    <t>P16</t>
-  </si>
-  <si>
-    <t>P15</t>
-  </si>
-  <si>
-    <t>P14</t>
-  </si>
-  <si>
-    <t>P13</t>
-  </si>
-  <si>
-    <t>P12</t>
-  </si>
-  <si>
-    <t>P11</t>
-  </si>
-  <si>
-    <t>P10</t>
-  </si>
-  <si>
-    <t>P0F</t>
-  </si>
-  <si>
-    <t>P0B</t>
-  </si>
-  <si>
-    <t>P0A</t>
-  </si>
-  <si>
-    <t>P09</t>
-  </si>
-  <si>
-    <t>P08</t>
-  </si>
-  <si>
-    <t>P07</t>
-  </si>
-  <si>
-    <t>P06</t>
-  </si>
-  <si>
-    <t>P05</t>
-  </si>
-  <si>
-    <t>P02</t>
-  </si>
-  <si>
-    <t>P03</t>
-  </si>
-  <si>
-    <t>P04</t>
-  </si>
-  <si>
     <t>ARRANQUE VENTILADORES</t>
   </si>
   <si>
@@ -181,42 +117,6 @@
   </si>
   <si>
     <t>COMPUERTA RECIRCULACION</t>
-  </si>
-  <si>
-    <t>P4D</t>
-  </si>
-  <si>
-    <t>P4C</t>
-  </si>
-  <si>
-    <t>P4B</t>
-  </si>
-  <si>
-    <t>P4A</t>
-  </si>
-  <si>
-    <t>P49</t>
-  </si>
-  <si>
-    <t>P48</t>
-  </si>
-  <si>
-    <t>P46</t>
-  </si>
-  <si>
-    <t>P45</t>
-  </si>
-  <si>
-    <t>P44</t>
-  </si>
-  <si>
-    <t>P43</t>
-  </si>
-  <si>
-    <t>P41</t>
-  </si>
-  <si>
-    <t>P42</t>
   </si>
   <si>
     <t>P00 HonHab</t>
@@ -368,7 +268,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -654,208 +554,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F23"/>
+  <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="47.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" t="s">
         <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -863,15 +773,15 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -879,15 +789,15 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
@@ -895,18 +805,10 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -916,209 +818,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" t="s">
-        <v>96</v>
-      </c>
-      <c r="F9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" t="s">
-        <v>94</v>
-      </c>
-      <c r="F11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" t="s">
-        <v>97</v>
-      </c>
-      <c r="F12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" t="s">
-        <v>98</v>
-      </c>
-      <c r="F13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" t="s">
-        <v>99</v>
-      </c>
-      <c r="F14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>